<commit_message>
work deep 01 2023-03-22
</commit_message>
<xml_diff>
--- a/015 VBA Programming/14-04-data-tables-one-variable.xlsx
+++ b/015 VBA Programming/14-04-data-tables-one-variable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web learning\015 VBA Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E868F6B-681E-42CF-B969-343BABB4137A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E5DBC1-CD80-4961-8D7C-9BA7ACA2181D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{67801036-0AA2-429B-B929-859D7C2219F4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>Data Tables: One Variable</t>
   </si>
@@ -512,8 +512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66B31A40-279F-4A5E-A73D-0CB5FEC63765}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,6 +521,7 @@
     <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
@@ -570,8 +571,13 @@
         <v>348.61487886678395</v>
       </c>
       <c r="D9" s="7"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="7"/>
+      <c r="E9" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="11">
+        <f>B6</f>
+        <v>348.61487886678395</v>
+      </c>
       <c r="G9" s="8"/>
       <c r="H9" s="7"/>
     </row>
@@ -580,8 +586,15 @@
         <v>0.01</v>
       </c>
       <c r="C10" s="11">
-        <f t="dataTable" ref="C10:C20" dt2D="0" dtr="0" r1="B4"/>
+        <f t="dataTable" ref="C10:C20" dt2D="0" dtr="0" r1="B4" ca="1"/>
         <v>337.65622330751347</v>
+      </c>
+      <c r="E10" s="10">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="dataTable" ref="F10:F20" dt2D="1" dtr="1" r1="B4" r2="B3" ca="1"/>
+        <v>Interest Rate</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -591,6 +604,12 @@
       <c r="C11" s="11">
         <v>338.74235982923778</v>
       </c>
+      <c r="E11" s="10">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="F11" t="str">
+        <v>Interest Rate</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" s="10">
@@ -599,6 +618,12 @@
       <c r="C12" s="11">
         <v>339.83066048347501</v>
       </c>
+      <c r="E12" s="10">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F12" t="str">
+        <v>Interest Rate</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" s="10">
@@ -607,6 +632,12 @@
       <c r="C13" s="11">
         <v>340.92112450204388</v>
       </c>
+      <c r="E13" s="10">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="F13" t="str">
+        <v>Interest Rate</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" s="10">
@@ -615,6 +646,12 @@
       <c r="C14" s="11">
         <v>342.01375110035013</v>
       </c>
+      <c r="E14" s="10">
+        <v>2E-3</v>
+      </c>
+      <c r="F14" t="str">
+        <v>Interest Rate</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" s="10">
@@ -623,6 +660,12 @@
       <c r="C15" s="11">
         <v>343.10853947741617</v>
       </c>
+      <c r="E15" s="10">
+        <v>2.2499999999999998E-3</v>
+      </c>
+      <c r="F15" t="str">
+        <v>Interest Rate</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" s="10">
@@ -631,40 +674,70 @@
       <c r="C16" s="11">
         <v>344.20548881590929</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E16" s="10">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F16" t="str">
+        <v>Interest Rate</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="10">
         <v>2.75E-2</v>
       </c>
       <c r="C17" s="11">
         <v>345.30459828217289</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E17" s="10">
+        <v>2.75E-2</v>
+      </c>
+      <c r="F17" t="str">
+        <v>Interest Rate</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="10">
         <v>0.03</v>
       </c>
       <c r="C18" s="11">
         <v>346.40586702625524</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E18" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="F18" t="str">
+        <v>Interest Rate</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="10">
         <v>3.2500000000000001E-2</v>
       </c>
       <c r="C19" s="11">
         <v>347.50929418194153</v>
       </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E19" s="10">
+        <v>3.2500000000000001E-2</v>
+      </c>
+      <c r="F19" t="str">
+        <v>Interest Rate</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="10">
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="C20" s="11">
         <v>348.61487886678395</v>
       </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E20" s="10">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="F20" t="str">
+        <v>Interest Rate</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="8"/>
     </row>
   </sheetData>

</xml_diff>